<commit_message>
[EXTRA SCRAPE] added more code from azure vm
</commit_message>
<xml_diff>
--- a/bin/sheets/main_db/teams/AUS/PlayerPerformance_3637.xlsx
+++ b/bin/sheets/main_db/teams/AUS/PlayerPerformance_3637.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Player Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ODI Batting" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="ODI Bowling" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ODI Batting Extra" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1909,6 +1908,7 @@
           <t>27</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>23/06/2012</t>
@@ -3256,6 +3256,7 @@
           <t>53</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
           <t>26/01/2015</t>
@@ -8021,543 +8022,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>MATCH_CODE</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>BATTING_POSITION</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NUM_4</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>NUM_6</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>PERCENT_RUNS_OF_TOTAL</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MAN_OF_MATCH</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>4423</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>25.97%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4429</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2.04%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>4430</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2.90%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4431</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7.87%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4435</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4436</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>4594</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>4597</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>19.58%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>4600</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>4601</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>38.98%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>4603</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6.10%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>4644</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>28.36%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>4645</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>13.00%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>4646</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>66.67%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>4647</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>4648</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2.56%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>4660</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>4663</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>4666</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>4732</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>8.55%</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>